<commit_message>
IO level of pins is 3.3V!
</commit_message>
<xml_diff>
--- a/doc/DAQad7606_bb.xlsx
+++ b/doc/DAQad7606_bb.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="111">
   <si>
     <t>Vdrive</t>
   </si>
@@ -403,6 +403,10 @@
       </rPr>
       <t>nput</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pin is 3.3v safe, do not put 5v on pins of beaglebone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -464,14 +468,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,7 +774,7 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,21 +801,21 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,22 +826,22 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>18</v>
@@ -885,11 +889,11 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -900,7 +904,7 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1">
@@ -919,7 +923,7 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="4"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1">
         <v>0</v>
       </c>
@@ -927,7 +931,9 @@
         <v>25</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1302,7 +1308,7 @@
       <c r="D25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>105</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1401,11 +1407,11 @@
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1491,7 +1497,7 @@
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B38" s="1">
@@ -1510,7 +1516,7 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="4"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="1">
         <v>0</v>
       </c>
@@ -1583,8 +1589,8 @@
       <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -1598,8 +1604,8 @@
       <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>

</xml_diff>

<commit_message>
pinmux compatible for BBB(eMMC)
</commit_message>
<xml_diff>
--- a/doc/DAQad7606_bb.xlsx
+++ b/doc/DAQad7606_bb.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="840" windowWidth="18615" windowHeight="7590" activeTab="1"/>
+    <workbookView xWindow="510" yWindow="840" windowWidth="18615" windowHeight="7590" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PIN" sheetId="1" r:id="rId1"/>
     <sheet name="AD7606-x" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="PIN set" sheetId="3" r:id="rId3"/>
+    <sheet name="PRU interrupt" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
@@ -24,8 +25,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>guoqiangxia</author>
+  </authors>
+  <commentList>
+    <comment ref="J24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>guoqiangxia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+default mode: direct connection, bit 0~16 all mapped out</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="169">
   <si>
     <t>Vdrive</t>
   </si>
@@ -520,6 +555,416 @@
         <family val="2"/>
       </rPr>
       <t>,2,5,6</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data0</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data1</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data2</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data3</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data4</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data5</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data6</t>
+  </si>
+  <si>
+    <t>echo "3e" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_data7</t>
+  </si>
+  <si>
+    <t>echo "5" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_vsync</t>
+  </si>
+  <si>
+    <t>echo "5" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_hsync</t>
+  </si>
+  <si>
+    <t>echo "5" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_pclk</t>
+  </si>
+  <si>
+    <t>echo "5" &gt;&gt; /sys/kernel/debug/omap_mux/lcd_ac_bias_en</t>
+  </si>
+  <si>
+    <r>
+      <t>GPIO1_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>GPIO1_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>GPIO1_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO1_15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>m335x</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpmc_ad13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPMC_AD12 </t>
+  </si>
+  <si>
+    <t>gpmc_ad15</t>
+  </si>
+  <si>
+    <t>gpmc_ad14</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ode 0</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>N beaglebone black P8_11 to P8_21 is used for eMMC</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRU composite  de-multiplexer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2 channels</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>apped to</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system interrupts 32 through 63</t>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>31[0:4]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>hannel number</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>31[5]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nable pulse on above channel number</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">So even for interrupt generation, I can still use r31.bit6 and r31.bit7 as output, PRU0 r31 can be used for </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pru0_r31_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ru0_r30_7</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ru0_r31_6</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pru0_r30_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ru0_r31_16</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P9_24</t>
+  </si>
+  <si>
+    <t>P9_25</t>
+  </si>
+  <si>
+    <t>P9_41B</t>
+  </si>
+  <si>
+    <t>mode 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uart1_txd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mcasp0_ahclkx </t>
+  </si>
+  <si>
+    <t>mode 6, input, disable pullup/down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode 5, output, enable pulldown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">cho "5" &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>/sys/kernel/debug/omap_mux/mcasp0_ahclkx</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P9_25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ight source on/off</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>cho "3e" &gt;&gt; /sys/kernel/debug/omap_mux/uart1_txd</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>9_24</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>otation home</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -528,7 +973,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -544,6 +989,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -595,6 +1053,51 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2105025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3074" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2105025" y="3476625"/>
+          <a:ext cx="7581900" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1106,6 +1609,12 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
+      <c r="L11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1"/>
@@ -1190,7 +1699,9 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:14">
@@ -1213,10 +1724,12 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1242,8 +1755,14 @@
       <c r="K17" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="M17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1269,8 +1788,14 @@
       <c r="K18" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1296,8 +1821,14 @@
       <c r="K19" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -1323,8 +1854,14 @@
       <c r="K20" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1347,7 +1884,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1364,11 +1901,20 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="I22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K22" t="s">
+        <v>156</v>
+      </c>
+      <c r="M22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -1385,11 +1931,17 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="I23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -1407,10 +1959,17 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="J24" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1431,7 +1990,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:13">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1444,7 +2003,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:13">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1457,7 +2016,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>110</v>
       </c>
@@ -1474,7 +2033,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:13">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1487,7 +2046,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1504,7 +2063,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:13">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1517,7 +2076,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:13">
       <c r="A32" s="5" t="s">
         <v>86</v>
       </c>
@@ -1849,6 +2408,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1856,7 +2416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1909,18 +2469,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="121.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2"/>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1">
+        <v>111110</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11">
+        <v>101</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>